<commit_message>
typo error in readme.md
</commit_message>
<xml_diff>
--- a/Front/pages/resources/contacts.xlsx
+++ b/Front/pages/resources/contacts.xlsx
@@ -512,12 +512,12 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nuevos</t>
+          <t>Baneados</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>

</xml_diff>